<commit_message>
Updating kernel density plot colors so null dist is black
</commit_message>
<xml_diff>
--- a/EcologicalNichePlots/KS_Tests.xlsx
+++ b/EcologicalNichePlots/KS_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RebeccaCohen/Documents/GitHub/HabitatModeling/EcologicalNichePlots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF16866-B8C4-A848-8254-CAD891AFC74A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BC4496-3621-7849-8701-3630354C0A8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52282028-A7E2-584D-B37E-C615246B22D1}"/>
+    <workbookView xWindow="4340" yWindow="460" windowWidth="24040" windowHeight="17040" activeTab="1" xr2:uid="{52282028-A7E2-584D-B37E-C615246B22D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Md Me" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="60">
   <si>
     <t>Chl0</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>Gm vs Gg @ HAT</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>**</t>
   </si>
 </sst>
 </file>
@@ -564,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C831003-7A88-1545-94C2-4E88EC912316}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:N4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,6 +760,199 @@
         <v>5.6500000000000002E-2</v>
       </c>
     </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -755,10 +960,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FC531F-1860-F240-9E5A-FB421E1603A4}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:N12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1201,6 +1406,451 @@
       </c>
       <c r="N12" s="1">
         <v>0.99850000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Getting rid of plots at wrong depth layer
</commit_message>
<xml_diff>
--- a/EcologicalNichePlots/KS_Tests.xlsx
+++ b/EcologicalNichePlots/KS_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RebeccaCohen/Documents/GitHub/HabitatModeling/EcologicalNichePlots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BC4496-3621-7849-8701-3630354C0A8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6F4E1C-9905-7E4D-ACAF-59FA9CD9D0AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="460" windowWidth="24040" windowHeight="17040" activeTab="1" xr2:uid="{52282028-A7E2-584D-B37E-C615246B22D1}"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="24400" windowHeight="17500" activeTab="3" xr2:uid="{52282028-A7E2-584D-B37E-C615246B22D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Md Me" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="60">
   <si>
     <t>Chl0</t>
   </si>
@@ -579,7 +579,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FC531F-1860-F240-9E5A-FB421E1603A4}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:J28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1860,10 +1860,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA77E5D-3B23-6743-A85E-7174BAC877BD}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:N1"/>
+      <selection activeCell="B15" sqref="B15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2176,6 +2176,325 @@
         <v>0.1469</v>
       </c>
     </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2183,10 +2502,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E8B3A9A-9648-CF43-83F6-904001254CBE}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3159,6 +3478,1961 @@
         <v>0.75860000000000005</v>
       </c>
     </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I34" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" t="s">
+        <v>43</v>
+      </c>
+      <c r="K34" t="s">
+        <v>44</v>
+      </c>
+      <c r="L34" t="s">
+        <v>45</v>
+      </c>
+      <c r="M34" t="s">
+        <v>46</v>
+      </c>
+      <c r="N34" t="s">
+        <v>47</v>
+      </c>
+      <c r="O34" t="s">
+        <v>48</v>
+      </c>
+      <c r="P34" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>50</v>
+      </c>
+      <c r="R34" t="s">
+        <v>51</v>
+      </c>
+      <c r="S34" t="s">
+        <v>52</v>
+      </c>
+      <c r="T34" t="s">
+        <v>53</v>
+      </c>
+      <c r="U34" t="s">
+        <v>54</v>
+      </c>
+      <c r="V34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="V38" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V39" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V40" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V41" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V42" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V43" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V46" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V47" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>3</v>
+      </c>
+      <c r="F49" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" t="s">
+        <v>32</v>
+      </c>
+      <c r="I49" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" t="s">
+        <v>33</v>
+      </c>
+      <c r="K49" t="s">
+        <v>9</v>
+      </c>
+      <c r="L49" t="s">
+        <v>34</v>
+      </c>
+      <c r="M49" t="s">
+        <v>11</v>
+      </c>
+      <c r="N49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N66" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>37</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N68" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>36</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N69" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" t="s">
+        <v>3</v>
+      </c>
+      <c r="F71" t="s">
+        <v>31</v>
+      </c>
+      <c r="G71" t="s">
+        <v>5</v>
+      </c>
+      <c r="H71" t="s">
+        <v>32</v>
+      </c>
+      <c r="I71" t="s">
+        <v>7</v>
+      </c>
+      <c r="J71" t="s">
+        <v>33</v>
+      </c>
+      <c r="K71" t="s">
+        <v>9</v>
+      </c>
+      <c r="L71" t="s">
+        <v>34</v>
+      </c>
+      <c r="M71" t="s">
+        <v>11</v>
+      </c>
+      <c r="N71" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>